<commit_message>
Lots of schematic updates. Started on layout a little too.
</commit_message>
<xml_diff>
--- a/Design/port peripheral mapping.xlsx
+++ b/Design/port peripheral mapping.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hydra\Documents\DipTrace\Projects\MakerPnPControl\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ACBF83-D847-49F5-98C7-B570E8FEE9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B012718D-815A-444C-B765-93DB265C8BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24675" yWindow="7410" windowWidth="25935" windowHeight="23445" xr2:uid="{C3A3646F-069D-4AE0-AC21-8ACD43A56D36}"/>
-    <workbookView xWindow="7755" yWindow="7755" windowWidth="43200" windowHeight="23445" activeTab="1" xr2:uid="{98E0C64B-CFC7-49D6-B59B-4E132D082277}"/>
+    <workbookView xWindow="7755" yWindow="7755" windowWidth="43200" windowHeight="23445" xr2:uid="{98E0C64B-CFC7-49D6-B59B-4E132D082277}"/>
   </bookViews>
   <sheets>
     <sheet name="UFBGA176+25 Ports" sheetId="5" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="768">
   <si>
     <t>Port</t>
   </si>
@@ -1817,9 +1817,6 @@
     <t>PWM Fan 4</t>
   </si>
   <si>
-    <t>PWM output 1</t>
-  </si>
-  <si>
     <t>PWM output 2</t>
   </si>
   <si>
@@ -1913,15 +1910,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>FPGA and MCU share a flash chip.  MCU must not drive signals when FPGA boots, SS needs to be correct on boot to tell FPGA how to use the SPI.</t>
-  </si>
-  <si>
-    <t>Flash is programmed by the MCU.</t>
-  </si>
-  <si>
-    <t>Flash can be used by the MCU after the FPGA has booted.</t>
-  </si>
-  <si>
     <t>Backup FPGA images, configuration data and other stuff can be stored on the flash.</t>
   </si>
   <si>
@@ -2225,12 +2213,6 @@
     <t>Column3</t>
   </si>
   <si>
-    <t>Hardware Pin for Buzzer + 6x PWM controlled outputs using DMA stream on GPIO Port G</t>
-  </si>
-  <si>
-    <t>PWM output 3</t>
-  </si>
-  <si>
     <t>FPGA generated clock</t>
   </si>
   <si>
@@ -2379,6 +2361,18 @@
   </si>
   <si>
     <t>For expansion port</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>FPGA and MCU share a flash chip.  MCU must not drive signals when FPGA boots, SS needs to be correct on boot to tell FPGA how to use the SPI, Flash WP and HOLD need to be correct too.</t>
+  </si>
+  <si>
+    <t>Flash is programmed by the MCU, via OCTOSPI.</t>
+  </si>
+  <si>
+    <t>Flash can be used by the MCU after the FPGA has booted, memory mapped if needed.</t>
   </si>
 </sst>
 </file>
@@ -2826,8 +2820,8 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,7 +3093,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C9" t="str">
         <f>'UFBFA176+25 Peripherals'!B81</f>
@@ -3108,7 +3102,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3158,7 +3152,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3210,57 +3204,57 @@
         <v>414</v>
       </c>
       <c r="I24" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>614</v>
+        <v>765</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>615</v>
+        <v>766</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>616</v>
+        <v>767</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -3276,8 +3270,8 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="1">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3873,9 +3867,6 @@
       <c r="B12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
-        <v>582</v>
-      </c>
       <c r="D12" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A12,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
         <v>NONE</v>
@@ -3937,7 +3928,7 @@
         <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A13,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
@@ -4062,9 +4053,6 @@
       <c r="B15" t="s">
         <v>103</v>
       </c>
-      <c r="C15" t="s">
-        <v>719</v>
-      </c>
       <c r="D15" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A15,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
         <v>NONE</v>
@@ -4126,7 +4114,7 @@
         <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>718</v>
+        <v>764</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A16,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
@@ -4628,7 +4616,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D28" s="1" t="str">
         <f>_xlfn.XLOOKUP($A28,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4640,7 +4628,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D29" s="1" t="str">
         <f>_xlfn.XLOOKUP($A29,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4652,7 +4640,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D30" s="1" t="str">
         <f>_xlfn.XLOOKUP($A30,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4664,7 +4652,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>_xlfn.XLOOKUP($A31,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4676,7 +4664,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="D32" s="1" t="str">
         <f>_xlfn.XLOOKUP($A32,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4688,7 +4676,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>_xlfn.XLOOKUP($A33,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4891,7 +4879,7 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D41" s="1" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A41,"_",D$37),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5318,7 +5306,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D55" s="1" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5331,7 +5319,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D56" s="1" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5347,7 +5335,7 @@
         <v>426</v>
       </c>
       <c r="C57" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="D57" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5363,7 +5351,7 @@
         <v>429</v>
       </c>
       <c r="C58" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="D58" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5383,13 +5371,13 @@
         <v>345</v>
       </c>
       <c r="E60" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="F60" t="s">
         <v>346</v>
       </c>
       <c r="G60" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="H60" t="s">
         <v>348</v>
@@ -5406,10 +5394,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="B61" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C61" t="s">
         <v>92</v>
@@ -5454,16 +5442,16 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="E62" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="F62" t="s">
         <v>347</v>
       </c>
       <c r="G62" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="H62" t="s">
         <v>352</v>
@@ -5485,13 +5473,13 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="B63" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C63" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="D63" s="1" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",D$62),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5615,7 +5603,7 @@
         <v>43</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D69" t="str" cm="1">
         <f t="array" ref="D69" xml:space="preserve"> IF(C69&lt;&gt;"",
@@ -5711,7 +5699,7 @@
         <v>98</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="D75" t="str" cm="1">
         <f t="array" ref="D75" xml:space="preserve"> IF(C75&lt;&gt;"",
@@ -5753,7 +5741,7 @@
         <v>102</v>
       </c>
       <c r="C78" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D78" t="str" cm="1">
         <f t="array" ref="D78" xml:space="preserve"> IF(C78&lt;&gt;"",
@@ -5769,7 +5757,7 @@
         <v>382</v>
       </c>
       <c r="C79" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D79" t="str" cm="1">
         <f t="array" ref="D79" xml:space="preserve"> IF(C79&lt;&gt;"",
@@ -5785,7 +5773,7 @@
         <v>100</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="D80" t="str" cm="1">
         <f t="array" ref="D80" xml:space="preserve"> IF(C80&lt;&gt;"",
@@ -5850,7 +5838,7 @@
         <v>111</v>
       </c>
       <c r="C88" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D88" s="1" t="str">
         <f>_xlfn.XLOOKUP($A88,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5865,7 +5853,7 @@
         <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D89" s="1" t="str">
         <f>_xlfn.XLOOKUP($A89,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5904,7 +5892,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="D93" s="1" t="e">
         <f>_xlfn.XLOOKUP($A93,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5913,7 +5901,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="D94" s="1" t="e">
         <f>_xlfn.XLOOKUP($A94,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5922,7 +5910,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="D95" s="1" t="e">
         <f>_xlfn.XLOOKUP($A95,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5931,7 +5919,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="D96" s="1" t="e">
         <f>_xlfn.XLOOKUP($A96,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5940,7 +5928,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="D97" s="1" t="e">
         <f>_xlfn.XLOOKUP($A97,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5949,7 +5937,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="D98" s="1" t="e">
         <f>_xlfn.XLOOKUP($A98,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5958,7 +5946,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="D99" s="1" t="e">
         <f>_xlfn.XLOOKUP($A99,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5967,7 +5955,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="D100" s="1" t="e">
         <f>_xlfn.XLOOKUP($A100,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -5976,10 +5964,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="C102" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="D102" s="1" t="str">
         <f>_xlfn.XLOOKUP($A102,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6019,39 +6007,39 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C107" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C108" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C109" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C110" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="C112" t="s">
         <v>128</v>
@@ -6059,7 +6047,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C113" t="s">
         <v>129</v>
@@ -6067,7 +6055,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="C114" t="s">
         <v>130</v>
@@ -6075,7 +6063,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="C115" t="s">
         <v>130</v>
@@ -6083,7 +6071,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="C116" t="s">
         <v>131</v>
@@ -6091,7 +6079,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="C117" t="s">
         <v>132</v>
@@ -6099,7 +6087,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C118" t="s">
         <v>127</v>
@@ -6107,7 +6095,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="C119" t="s">
         <v>126</v>
@@ -6217,7 +6205,7 @@
         <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>139</v>
@@ -6273,7 +6261,7 @@
         <v>142</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>139</v>
@@ -6369,7 +6357,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>139</v>
@@ -6408,7 +6396,7 @@
         <v>142</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>139</v>
@@ -6884,7 +6872,7 @@
         <v>310</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>139</v>
@@ -7004,7 +6992,7 @@
         <v>142</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>139</v>
@@ -7031,7 +7019,7 @@
         <v>142</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>139</v>
@@ -7100,7 +7088,7 @@
         <v>93</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>139</v>
@@ -7118,7 +7106,7 @@
         <v>139</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -7141,7 +7129,7 @@
         <v>142</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>139</v>
@@ -7212,7 +7200,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>139</v>
@@ -7280,7 +7268,7 @@
         <v>142</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>139</v>
@@ -7307,7 +7295,7 @@
         <v>142</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>139</v>
@@ -7529,7 +7517,7 @@
         <v>139</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>1</v>
@@ -7639,7 +7627,7 @@
         <v>139</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>1</v>
@@ -7722,7 +7710,7 @@
         <v>139</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>1</v>
@@ -7787,7 +7775,7 @@
         <v>105</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>139</v>
@@ -7886,7 +7874,7 @@
         <v>139</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="I64" s="1" t="b">
         <v>1</v>
@@ -8320,7 +8308,7 @@
         <v>139</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="I80" s="1" t="b">
         <v>1</v>
@@ -8457,7 +8445,7 @@
         <v>139</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="I85" s="1" t="b">
         <v>1</v>
@@ -8576,7 +8564,7 @@
         <v>265</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>139</v>
@@ -8621,7 +8609,7 @@
         <v>139</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="I91" s="1" t="b">
         <v>1</v>
@@ -8677,7 +8665,7 @@
         <v>139</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="I93" s="1" t="b">
         <v>1</v>
@@ -8742,7 +8730,7 @@
         <v>106</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>139</v>
@@ -8877,7 +8865,7 @@
         <v>62</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>139</v>
@@ -8976,7 +8964,7 @@
         <v>139</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="I104" s="1" t="b">
         <v>1</v>
@@ -9005,7 +8993,7 @@
         <v>139</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="I105" s="1" t="b">
         <v>1</v>
@@ -9034,7 +9022,7 @@
         <v>139</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="I106" s="1" t="b">
         <v>1</v>
@@ -9045,7 +9033,7 @@
         <v>119</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>139</v>
@@ -9063,7 +9051,7 @@
         <v>139</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="I107" s="1" t="b">
         <v>1</v>
@@ -9119,7 +9107,7 @@
         <v>139</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="I109" s="1" t="b">
         <v>1</v>
@@ -9130,7 +9118,7 @@
         <v>122</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>139</v>
@@ -9148,7 +9136,7 @@
         <v>139</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="I110" s="1" t="b">
         <v>1</v>
@@ -9225,7 +9213,7 @@
         <v>142</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>139</v>
@@ -9240,7 +9228,7 @@
         <v>292</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>139</v>
@@ -9267,7 +9255,7 @@
         <v>294</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>139</v>
@@ -9294,7 +9282,7 @@
         <v>53</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>139</v>
@@ -9404,7 +9392,7 @@
         <v>124</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>139</v>
@@ -9431,7 +9419,7 @@
         <v>296</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>139</v>
@@ -9458,7 +9446,7 @@
         <v>125</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>139</v>
@@ -9476,7 +9464,7 @@
         <v>139</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="I122" s="1" t="b">
         <v>1</v>
@@ -9750,7 +9738,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="I132" s="1" t="b">
         <v>1</v>
@@ -10271,7 +10259,7 @@
         <v>479</v>
       </c>
       <c r="E29" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="G29" t="s">
         <v>536</v>
@@ -10400,7 +10388,7 @@
         <v>92</v>
       </c>
       <c r="G35" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="J35" t="s">
         <v>554</v>
@@ -10505,13 +10493,13 @@
         <v>478</v>
       </c>
       <c r="E40" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="G40" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="H40" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="J40" t="s">
         <v>554</v>
@@ -10550,13 +10538,13 @@
         <v>478</v>
       </c>
       <c r="E42" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="G42" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="H42" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="J42" t="s">
         <v>554</v>
@@ -11444,8 +11432,8 @@
   <dimension ref="A1:H154"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A100" workbookViewId="1">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11478,10 +11466,10 @@
         <v>542</v>
       </c>
       <c r="G1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="H1" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -12006,7 +11994,7 @@
         <v>566</v>
       </c>
       <c r="F30" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -12027,7 +12015,7 @@
         <v>566</v>
       </c>
       <c r="F31" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -12048,7 +12036,7 @@
         <v>566</v>
       </c>
       <c r="F32" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -12069,7 +12057,7 @@
         <v>566</v>
       </c>
       <c r="F33" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -12090,7 +12078,7 @@
         <v>566</v>
       </c>
       <c r="F34" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -12111,7 +12099,7 @@
         <v>566</v>
       </c>
       <c r="F35" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -12132,7 +12120,7 @@
         <v>566</v>
       </c>
       <c r="F36" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -12153,7 +12141,7 @@
         <v>566</v>
       </c>
       <c r="F37" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -12174,7 +12162,7 @@
         <v>566</v>
       </c>
       <c r="F38" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -12195,7 +12183,7 @@
         <v>566</v>
       </c>
       <c r="F39" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -12216,7 +12204,7 @@
         <v>566</v>
       </c>
       <c r="F40" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -12237,7 +12225,7 @@
         <v>566</v>
       </c>
       <c r="F41" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -12258,7 +12246,7 @@
         <v>566</v>
       </c>
       <c r="F42" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -12279,7 +12267,7 @@
         <v>566</v>
       </c>
       <c r="F43" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -12300,7 +12288,7 @@
         <v>566</v>
       </c>
       <c r="F44" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -12321,7 +12309,7 @@
         <v>566</v>
       </c>
       <c r="F45" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -12342,7 +12330,7 @@
         <v>566</v>
       </c>
       <c r="F46" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -12363,7 +12351,7 @@
         <v>566</v>
       </c>
       <c r="F47" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -12384,7 +12372,7 @@
         <v>566</v>
       </c>
       <c r="F48" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -12405,7 +12393,7 @@
         <v>566</v>
       </c>
       <c r="F49" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -12426,7 +12414,7 @@
         <v>566</v>
       </c>
       <c r="F50" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -12447,7 +12435,7 @@
         <v>566</v>
       </c>
       <c r="F51" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -12468,7 +12456,7 @@
         <v>566</v>
       </c>
       <c r="F52" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -12489,7 +12477,7 @@
         <v>566</v>
       </c>
       <c r="F53" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -12510,7 +12498,7 @@
         <v>566</v>
       </c>
       <c r="F54" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -12531,7 +12519,7 @@
         <v>566</v>
       </c>
       <c r="F55" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -12552,7 +12540,7 @@
         <v>566</v>
       </c>
       <c r="F56" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -12573,7 +12561,7 @@
         <v>566</v>
       </c>
       <c r="F57" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -12594,7 +12582,7 @@
         <v>566</v>
       </c>
       <c r="F58" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -12615,7 +12603,7 @@
         <v>566</v>
       </c>
       <c r="F59" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -12636,7 +12624,7 @@
         <v>566</v>
       </c>
       <c r="F60" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -12657,7 +12645,7 @@
         <v>566</v>
       </c>
       <c r="F61" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -12678,7 +12666,7 @@
         <v>566</v>
       </c>
       <c r="F62" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -12699,7 +12687,7 @@
         <v>566</v>
       </c>
       <c r="F63" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -12720,7 +12708,7 @@
         <v>566</v>
       </c>
       <c r="F64" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -12741,7 +12729,7 @@
         <v>566</v>
       </c>
       <c r="F65" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -12762,7 +12750,7 @@
         <v>566</v>
       </c>
       <c r="F66" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -12783,7 +12771,7 @@
         <v>566</v>
       </c>
       <c r="F67" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -12804,7 +12792,7 @@
         <v>566</v>
       </c>
       <c r="F68" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -12825,7 +12813,7 @@
         <v>566</v>
       </c>
       <c r="F69" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -12846,7 +12834,7 @@
         <v>566</v>
       </c>
       <c r="F70" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -12867,7 +12855,7 @@
         <v>566</v>
       </c>
       <c r="F71" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -12888,7 +12876,7 @@
         <v>566</v>
       </c>
       <c r="F72" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -12909,7 +12897,7 @@
         <v>566</v>
       </c>
       <c r="F73" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -12930,7 +12918,7 @@
         <v>566</v>
       </c>
       <c r="F74" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -12951,7 +12939,7 @@
         <v>566</v>
       </c>
       <c r="F75" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -12972,7 +12960,7 @@
         <v>566</v>
       </c>
       <c r="F76" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -12993,7 +12981,7 @@
         <v>566</v>
       </c>
       <c r="F77" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -13014,7 +13002,7 @@
         <v>566</v>
       </c>
       <c r="F78" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -13035,7 +13023,7 @@
         <v>566</v>
       </c>
       <c r="F79" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -13056,7 +13044,7 @@
         <v>566</v>
       </c>
       <c r="F80" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -13077,7 +13065,7 @@
         <v>566</v>
       </c>
       <c r="F81" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -13098,7 +13086,7 @@
         <v>566</v>
       </c>
       <c r="F82" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -13119,7 +13107,7 @@
         <v>566</v>
       </c>
       <c r="F83" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -13140,7 +13128,7 @@
         <v>566</v>
       </c>
       <c r="F84" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -13161,7 +13149,7 @@
         <v>566</v>
       </c>
       <c r="F85" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -13182,7 +13170,7 @@
         <v>566</v>
       </c>
       <c r="F86" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -13203,7 +13191,7 @@
         <v>566</v>
       </c>
       <c r="F87" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -13224,7 +13212,7 @@
         <v>566</v>
       </c>
       <c r="F88" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -13245,7 +13233,7 @@
         <v>566</v>
       </c>
       <c r="F89" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -13266,7 +13254,7 @@
         <v>566</v>
       </c>
       <c r="F90" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -13287,7 +13275,7 @@
         <v>566</v>
       </c>
       <c r="F91" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -13308,7 +13296,7 @@
         <v>566</v>
       </c>
       <c r="F92" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -13329,7 +13317,7 @@
         <v>566</v>
       </c>
       <c r="F93" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -13905,13 +13893,13 @@
         <v>ENCODERX_A</v>
       </c>
       <c r="C130" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E130" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="F130" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -13923,13 +13911,13 @@
         <v>ENCODERX_B</v>
       </c>
       <c r="C131" t="s">
+        <v>622</v>
+      </c>
+      <c r="E131" t="s">
+        <v>624</v>
+      </c>
+      <c r="F131" t="s">
         <v>626</v>
-      </c>
-      <c r="E131" t="s">
-        <v>628</v>
-      </c>
-      <c r="F131" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -13941,13 +13929,13 @@
         <v>ENCODERX_Z</v>
       </c>
       <c r="C132" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E132" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="F132" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -13959,13 +13947,13 @@
         <v>ENCODERX_A</v>
       </c>
       <c r="C133" t="s">
+        <v>621</v>
+      </c>
+      <c r="E133" t="s">
         <v>625</v>
       </c>
-      <c r="E133" t="s">
-        <v>629</v>
-      </c>
       <c r="F133" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -13977,13 +13965,13 @@
         <v>ENCODERX_B</v>
       </c>
       <c r="C134" t="s">
+        <v>622</v>
+      </c>
+      <c r="E134" t="s">
+        <v>625</v>
+      </c>
+      <c r="F134" t="s">
         <v>626</v>
-      </c>
-      <c r="E134" t="s">
-        <v>629</v>
-      </c>
-      <c r="F134" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -13995,13 +13983,13 @@
         <v>ENCODERX_Z</v>
       </c>
       <c r="C135" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E135" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F135" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -14013,10 +14001,10 @@
         <v>DIGITAL_IN_5</v>
       </c>
       <c r="C136" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F136" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -14028,10 +14016,10 @@
         <v>DIGITAL_IN_6</v>
       </c>
       <c r="C137" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F137" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -14043,10 +14031,10 @@
         <v>DIGITAL_IN_7</v>
       </c>
       <c r="C138" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F138" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -14058,10 +14046,10 @@
         <v>DIGITAL_IN_8</v>
       </c>
       <c r="C139" t="s">
+        <v>599</v>
+      </c>
+      <c r="F139" t="s">
         <v>600</v>
-      </c>
-      <c r="F139" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -14073,10 +14061,10 @@
         <v>OPTO_OUT_1</v>
       </c>
       <c r="C140" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F140" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -14088,10 +14076,10 @@
         <v>OPTO_OUT_2</v>
       </c>
       <c r="C141" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F141" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -14103,10 +14091,10 @@
         <v>OPTO_IN_1</v>
       </c>
       <c r="C142" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F142" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -14118,10 +14106,10 @@
         <v>OPTO_IN_2</v>
       </c>
       <c r="C143" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F143" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -14136,7 +14124,7 @@
         <v>160</v>
       </c>
       <c r="E144" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -14148,10 +14136,10 @@
         <v>EXTI10_STEPPERS</v>
       </c>
       <c r="C145" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E145" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -14166,7 +14154,7 @@
         <v>420</v>
       </c>
       <c r="E146" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -14174,13 +14162,13 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="E147" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="F147" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -14192,13 +14180,13 @@
         <v>FPGA_SPI_CS</v>
       </c>
       <c r="C148" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E148" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F148" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -14210,13 +14198,13 @@
         <v>FPGA_SPI_SCK</v>
       </c>
       <c r="C149" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E149" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F149" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -14228,13 +14216,13 @@
         <v>FPGA_SPI_MISO</v>
       </c>
       <c r="C150" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E150" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F150" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -14246,13 +14234,13 @@
         <v>FPGA_SPI_MOSI</v>
       </c>
       <c r="C151" t="s">
+        <v>586</v>
+      </c>
+      <c r="E151" t="s">
         <v>587</v>
       </c>
-      <c r="E151" t="s">
-        <v>588</v>
-      </c>
       <c r="F151" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Further changes to support conditional memory mapping of the FLASH, the WIFI, the FPGA (again) or a device on the expansion port.
</commit_message>
<xml_diff>
--- a/Design/port peripheral mapping.xlsx
+++ b/Design/port peripheral mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hydra\Documents\DipTrace\Projects\MakerPnPControl\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA2C5C-6431-4814-B79C-38FC18B9897E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DCEB7E-A361-4B3B-B04A-956741318638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16305" yWindow="10050" windowWidth="19560" windowHeight="20535" activeTab="1" xr2:uid="{C3A3646F-069D-4AE0-AC21-8ACD43A56D36}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PORT_PINS!$A$11:$I$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'UFBGA176+25 GPIOs'!$A$1:$I$133</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'UFBFA176+25 Peripherals'!$A$1:$O$117</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'UFBFA176+25 Peripherals'!$A$1:$O$122</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'UFBGA176+25 GPIOs'!$A$1:$H$133</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="787">
   <si>
     <t>Port</t>
   </si>
@@ -2173,9 +2173,6 @@
     <t>Column3</t>
   </si>
   <si>
-    <t>EXTI15_RESERVED</t>
-  </si>
-  <si>
     <t>ADC3_INP10</t>
   </si>
   <si>
@@ -2287,18 +2284,9 @@
     <t>OCTOSPI2</t>
   </si>
   <si>
-    <t>memory mapped</t>
-  </si>
-  <si>
-    <t>FLASH</t>
-  </si>
-  <si>
     <t>Muxed between ports</t>
   </si>
   <si>
-    <t>For expansion port</t>
-  </si>
-  <si>
     <t>FPGA and MCU share a flash chip.  MCU must not drive signals when FPGA boots, SS needs to be correct on boot to tell FPGA how to use the SPI, Flash WP and HOLD need to be correct too.</t>
   </si>
   <si>
@@ -2371,9 +2359,6 @@
     <t>OUT2</t>
   </si>
   <si>
-    <t>Spare</t>
-  </si>
-  <si>
     <t>DIGITAL_IN_3</t>
   </si>
   <si>
@@ -2386,19 +2371,64 @@
     <t>Head communication (RS422, no flow control)</t>
   </si>
   <si>
-    <t xml:space="preserve">SPARE </t>
-  </si>
-  <si>
     <t>Head/Feeder communications</t>
   </si>
   <si>
     <t>Port communications</t>
   </si>
   <si>
-    <t xml:space="preserve">Spare </t>
-  </si>
-  <si>
     <t>Need 2x SW NSS for either SPI1 or SPI6</t>
+  </si>
+  <si>
+    <t>WIFI</t>
+  </si>
+  <si>
+    <t>EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>Device only, connected to an on-board USB hub</t>
+  </si>
+  <si>
+    <t>WIFI + EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>Port 2 / EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>Port 4 / EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>Port 1 / EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>Port 3 / EXPANSION PORT</t>
+  </si>
+  <si>
+    <t>OCTOSPI2_NCS_2</t>
+  </si>
+  <si>
+    <t>OCTOSPI2_NCS_3</t>
+  </si>
+  <si>
+    <t>FLASH - NCS to flash</t>
+  </si>
+  <si>
+    <t>EXPANSION_PORT</t>
+  </si>
+  <si>
+    <t>conditionally memory mapped</t>
+  </si>
+  <si>
+    <t>permanently memory mapped</t>
+  </si>
+  <si>
+    <t>Devices on expansion port can trigger MCU action since the FPGA is an IO expander</t>
+  </si>
+  <si>
+    <t>EXTI15_FPGA_RESERVED_OCTOSPI2_NCS_4</t>
+  </si>
+  <si>
+    <t>^ NOTE: all OCTOSPI_NCS_x pins are on EXTI15 pin Px15 so use here is flexible</t>
   </si>
 </sst>
 </file>
@@ -2844,7 +2874,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,7 +3149,7 @@
         <v>690</v>
       </c>
       <c r="C9" t="str">
-        <f>'UFBFA176+25 Peripherals'!B90</f>
+        <f>'UFBFA176+25 Peripherals'!B94</f>
         <v>0,1,2,3,4,5,6,7,8,9,13,14,15</v>
       </c>
     </row>
@@ -3237,17 +3267,17 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3288,17 +3318,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB4DCCF-6249-4668-B225-7F06A2FCE957}">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4071,7 +4102,7 @@
         <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A15,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
@@ -4134,7 +4165,7 @@
         <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>767</v>
+        <v>775</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A16,"_",D$2),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133,"NONE")</f>
@@ -4323,7 +4354,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>709</v>
+        <v>708</v>
+      </c>
+      <c r="C20" t="s">
+        <v>776</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>_xlfn.XLOOKUP($A20,'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4335,7 +4369,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>710</v>
+        <v>709</v>
+      </c>
+      <c r="C21" t="s">
+        <v>777</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>_xlfn.XLOOKUP($A21,'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4353,10 +4390,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="E23" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="F23" t="s">
         <v>94</v>
@@ -4366,6 +4403,9 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>771</v>
       </c>
       <c r="D24" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A24,"_",D$23),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4432,7 +4472,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>750</v>
+        <v>746</v>
+      </c>
+      <c r="C27" t="s">
+        <v>773</v>
       </c>
       <c r="D27" s="1" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A27,"_",D$26),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4491,7 +4534,7 @@
       <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="1" t="str">
@@ -4551,7 +4594,7 @@
       <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="1" t="str">
@@ -4611,7 +4654,7 @@
       <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="1" t="str">
@@ -4671,7 +4714,7 @@
       <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="1" t="str">
@@ -4729,7 +4772,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D32" s="1" t="e">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A32,"_",D$26),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4784,20 +4827,23 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>752</v>
+        <v>748</v>
+      </c>
+      <c r="C35" t="s">
+        <v>770</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>_xlfn.XLOOKUP($A35,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4807,9 +4853,12 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>753</v>
+        <v>749</v>
+      </c>
+      <c r="C36" t="s">
+        <v>771</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>_xlfn.XLOOKUP($A36,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4819,7 +4868,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>685</v>
       </c>
@@ -4831,7 +4880,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>684</v>
       </c>
@@ -4843,7 +4892,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>688</v>
       </c>
@@ -4855,7 +4904,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>686</v>
       </c>
@@ -4867,9 +4916,12 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>708</v>
+        <v>707</v>
+      </c>
+      <c r="C41" t="s">
+        <v>770</v>
       </c>
       <c r="D41" s="1" t="e">
         <f>_xlfn.XLOOKUP($A41,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4879,9 +4931,12 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>706</v>
+        <v>705</v>
+      </c>
+      <c r="C42" t="s">
+        <v>771</v>
       </c>
       <c r="D42" s="1" t="e">
         <f>_xlfn.XLOOKUP($A42,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -4891,13 +4946,13 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>407</v>
       </c>
@@ -4909,450 +4964,240 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D45" s="1"/>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E46" t="s">
+        <v>734</v>
+      </c>
+      <c r="F46" t="s">
+        <v>341</v>
+      </c>
+      <c r="G46" t="s">
+        <v>732</v>
+      </c>
+      <c r="H46" t="s">
+        <v>343</v>
+      </c>
+      <c r="I46" t="s">
+        <v>344</v>
+      </c>
+      <c r="J46" t="s">
+        <v>345</v>
+      </c>
+      <c r="K46" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>736</v>
+      </c>
+      <c r="B47" t="s">
+        <v>783</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG6</v>
+      </c>
+      <c r="F47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",F$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PF10</v>
+      </c>
+      <c r="G47" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",G$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",H$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD11</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",I$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD12</v>
+      </c>
+      <c r="J47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",J$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC2</v>
+      </c>
+      <c r="K47" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",K$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD13</v>
+      </c>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="E48" t="s">
+        <v>735</v>
+      </c>
+      <c r="F48" t="s">
+        <v>342</v>
+      </c>
+      <c r="G48" t="s">
+        <v>732</v>
+      </c>
+      <c r="H48" t="s">
+        <v>347</v>
+      </c>
+      <c r="I48" t="s">
+        <v>348</v>
+      </c>
+      <c r="J48" t="s">
+        <v>349</v>
+      </c>
+      <c r="K48" t="s">
+        <v>350</v>
+      </c>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>737</v>
+      </c>
+      <c r="B49" t="s">
+        <v>782</v>
+      </c>
+      <c r="C49" t="s">
+        <v>780</v>
+      </c>
+      <c r="D49" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",D$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",E$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG12</v>
+      </c>
+      <c r="F49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",F$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PF4</v>
+      </c>
+      <c r="G49" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",G$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",H$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD4</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",I$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH3</v>
+      </c>
+      <c r="J49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",J$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC3</v>
+      </c>
+      <c r="K49" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",K$48),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE10</v>
+      </c>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>778</v>
+      </c>
+      <c r="B50" t="s">
+        <v>782</v>
+      </c>
+      <c r="C50" t="s">
+        <v>770</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A50,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>779</v>
+      </c>
+      <c r="B51" t="s">
+        <v>782</v>
+      </c>
+      <c r="C51" t="s">
+        <v>781</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A51,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B52" t="s">
+        <v>782</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A52,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC15-OSC32_OUT</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>786</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>320</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E54" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>322</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C55" t="s">
         <v>323</v>
       </c>
-      <c r="D47" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A47,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="D55" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>PA10</v>
       </c>
-      <c r="E47" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A47,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="E55" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>PA9</v>
-      </c>
-      <c r="H47" t="str" cm="1">
-        <f t="array" ref="H47">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D47:G47),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>10,9</v>
-      </c>
-      <c r="I47" t="str" cm="1">
-        <f t="array" ref="I47">IF(
-    H47="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H47, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H47, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H47, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H47, ","))))
-        )
-    )
-)</f>
-        <v>9,10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" t="s">
-        <v>324</v>
-      </c>
-      <c r="D48" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A48,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD6</v>
-      </c>
-      <c r="E48" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A48,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD5</v>
-      </c>
-      <c r="H48" t="str" cm="1">
-        <f t="array" ref="H48">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D48:G48),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>6,5</v>
-      </c>
-      <c r="I48" t="str" cm="1">
-        <f t="array" ref="I48">IF(
-    H48="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H48, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H48, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H48, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H48, ","))))
-        )
-    )
-)</f>
-        <v>5,6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" t="s">
-        <v>325</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A49,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD9</v>
-      </c>
-      <c r="E49" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A49,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD8</v>
-      </c>
-      <c r="H49" t="str" cm="1">
-        <f t="array" ref="H49">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D49:G49),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>9,8</v>
-      </c>
-      <c r="I49" t="str" cm="1">
-        <f t="array" ref="I49">IF(
-    H49="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H49, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H49, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H49, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H49, ","))))
-        )
-    )
-)</f>
-        <v>8,9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" t="s">
-        <v>771</v>
-      </c>
-      <c r="D50" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A50,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD0</v>
-      </c>
-      <c r="E50" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A50,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD1</v>
-      </c>
-      <c r="H50" t="str" cm="1">
-        <f t="array" ref="H50">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D50:G50),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>0,1</v>
-      </c>
-      <c r="I50" t="str" cm="1">
-        <f t="array" ref="I50">IF(
-    H50="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H50, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H50, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H50, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H50, ","))))
-        )
-    )
-)</f>
-        <v>0,1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" t="s">
-        <v>326</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A51,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD2</v>
-      </c>
-      <c r="E51" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A51,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC12</v>
-      </c>
-      <c r="H51" t="str" cm="1">
-        <f t="array" ref="H51">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D51:G51),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>2,12</v>
-      </c>
-      <c r="I51" t="str" cm="1">
-        <f t="array" ref="I51">IF(
-    H51="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H51, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H51, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H51, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H51, ","))))
-        )
-    )
-)</f>
-        <v>2,12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>772</v>
-      </c>
-      <c r="D52" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A52,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG9</v>
-      </c>
-      <c r="E52" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A52,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG14</v>
-      </c>
-      <c r="H52" t="str" cm="1">
-        <f t="array" ref="H52">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D52:G52),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>9,14</v>
-      </c>
-      <c r="I52" t="str" cm="1">
-        <f t="array" ref="I52">IF(
-    H52="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H52, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H52, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H52, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H52, ","))))
-        )
-    )
-)</f>
-        <v>9,14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" t="s">
-        <v>328</v>
-      </c>
-      <c r="D53" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A53,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE7</v>
-      </c>
-      <c r="E53" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A53,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE8</v>
-      </c>
-      <c r="H53" t="str" cm="1">
-        <f t="array" ref="H53">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D53:G53),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>7,8</v>
-      </c>
-      <c r="I53" t="str" cm="1">
-        <f t="array" ref="I53">IF(
-    H53="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H53, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H53, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H53, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H53, ","))))
-        )
-    )
-)</f>
-        <v>7,8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" t="s">
-        <v>329</v>
-      </c>
-      <c r="D54" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A54,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE0</v>
-      </c>
-      <c r="E54" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A54,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE1</v>
-      </c>
-      <c r="H54" t="str" cm="1">
-        <f t="array" ref="H54">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D54:G54),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>0,1</v>
-      </c>
-      <c r="I54" t="str" cm="1">
-        <f t="array" ref="I54">IF(
-    H54="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H54, ","))))
-        )
-    )
-)</f>
-        <v>0,1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" t="s">
-        <v>327</v>
-      </c>
-      <c r="D55" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG0</v>
-      </c>
-      <c r="E55" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG1</v>
       </c>
       <c r="H55" t="str" cm="1">
         <f t="array" ref="H55">_xlfn.LET(
@@ -5373,7 +5218,7 @@
         ""
     )
 )</f>
-        <v>0,1</v>
+        <v>10,9</v>
       </c>
       <c r="I55" t="str" cm="1">
         <f t="array" ref="I55">IF(
@@ -5388,23 +5233,23 @@
         )
     )
 )</f>
-        <v>0,1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9,10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>380</v>
+        <v>324</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",D$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE2</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD6</v>
       </c>
       <c r="E56" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",E$46),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE3</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD5</v>
       </c>
       <c r="H56" t="str" cm="1">
         <f t="array" ref="H56">_xlfn.LET(
@@ -5425,7 +5270,7 @@
         ""
     )
 )</f>
-        <v>2,3</v>
+        <v>6,5</v>
       </c>
       <c r="I56" t="str" cm="1">
         <f t="array" ref="I56">IF(
@@ -5440,378 +5285,577 @@
         )
     )
 )</f>
+        <v>5,6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" t="s">
+        <v>325</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD9</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD8</v>
+      </c>
+      <c r="H57" t="str" cm="1">
+        <f t="array" ref="H57">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D57:G57),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>9,8</v>
+      </c>
+      <c r="I57" t="str" cm="1">
+        <f t="array" ref="I57">IF(
+    H57="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H57, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H57, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H57, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H57, ","))))
+        )
+    )
+)</f>
+        <v>8,9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>766</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD0</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD1</v>
+      </c>
+      <c r="H58" t="str" cm="1">
+        <f t="array" ref="H58">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D58:G58),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+      <c r="I58" t="str" cm="1">
+        <f t="array" ref="I58">IF(
+    H58="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H58, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H58, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H58, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H58, ","))))
+        )
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>326</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD2</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC12</v>
+      </c>
+      <c r="H59" t="str" cm="1">
+        <f t="array" ref="H59">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D59:G59),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>2,12</v>
+      </c>
+      <c r="I59" t="str" cm="1">
+        <f t="array" ref="I59">IF(
+    H59="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H59, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H59, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H59, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H59, ","))))
+        )
+    )
+)</f>
+        <v>2,12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" t="s">
+        <v>771</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG9</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG14</v>
+      </c>
+      <c r="H60" t="str" cm="1">
+        <f t="array" ref="H60">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D60:G60),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>9,14</v>
+      </c>
+      <c r="I60" t="str" cm="1">
+        <f t="array" ref="I60">IF(
+    H60="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H60, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H60, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H60, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H60, ","))))
+        )
+    )
+)</f>
+        <v>9,14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>328</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE7</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE8</v>
+      </c>
+      <c r="H61" t="str" cm="1">
+        <f t="array" ref="H61">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D61:G61),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>7,8</v>
+      </c>
+      <c r="I61" t="str" cm="1">
+        <f t="array" ref="I61">IF(
+    H61="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H61, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H61, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H61, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H61, ","))))
+        )
+    )
+)</f>
+        <v>7,8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" t="s">
+        <v>329</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE0</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE1</v>
+      </c>
+      <c r="H62" t="str" cm="1">
+        <f t="array" ref="H62">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D62:G62),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+      <c r="I62" t="str" cm="1">
+        <f t="array" ref="I62">IF(
+    H62="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H62, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H62, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H62, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H62, ","))))
+        )
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>327</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG0</v>
+      </c>
+      <c r="E63" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG1</v>
+      </c>
+      <c r="H63" t="str" cm="1">
+        <f t="array" ref="H63">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D63:G63),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+      <c r="I63" t="str" cm="1">
+        <f t="array" ref="I63">IF(
+    H63="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H63, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H63, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H63, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H63, ","))))
+        )
+    )
+)</f>
+        <v>0,1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" t="s">
+        <v>380</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE2</v>
+      </c>
+      <c r="E64" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE3</v>
+      </c>
+      <c r="H64" t="str" cm="1">
+        <f t="array" ref="H64">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D64:G64),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
         <v>2,3</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+      <c r="I64" t="str" cm="1">
+        <f t="array" ref="I64">IF(
+    H64="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H64, ","))))
+        )
+    )
+)</f>
+        <v>2,3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>320</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E66" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>416</v>
-      </c>
-      <c r="C59" t="s">
-        <v>774</v>
-      </c>
-      <c r="D59" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",D$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH14</v>
-      </c>
-      <c r="E59" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",E$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>417</v>
-      </c>
-      <c r="D60" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",D$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E60" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",E$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>418</v>
-      </c>
-      <c r="C61" t="s">
-        <v>773</v>
-      </c>
-      <c r="D61" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",D$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG10</v>
-      </c>
-      <c r="E61" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",E$58),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>420</v>
-      </c>
-      <c r="E63" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>694</v>
-      </c>
-      <c r="D64" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",D$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E64" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",E$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>695</v>
-      </c>
-      <c r="C65" t="s">
-        <v>741</v>
-      </c>
-      <c r="D65" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A65,"_",D$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH5</v>
-      </c>
-      <c r="E65" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A65,"_",E$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>419</v>
-      </c>
-      <c r="C66" t="s">
-        <v>742</v>
-      </c>
-      <c r="D66" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A66,"_",D$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH8</v>
-      </c>
-      <c r="E66" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A66,"_",E$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH7</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>422</v>
-      </c>
-      <c r="D67" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",D$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>416</v>
+      </c>
+      <c r="C67" t="s">
+        <v>768</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH14</v>
+      </c>
+      <c r="E67" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>417</v>
+      </c>
+      <c r="D68" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
-      <c r="E67" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",E$63),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="E68" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D69" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E69" t="s">
-        <v>735</v>
-      </c>
-      <c r="F69" t="s">
-        <v>341</v>
-      </c>
-      <c r="G69" t="s">
-        <v>733</v>
-      </c>
-      <c r="H69" t="s">
-        <v>343</v>
-      </c>
-      <c r="I69" t="s">
-        <v>344</v>
-      </c>
-      <c r="J69" t="s">
-        <v>345</v>
-      </c>
-      <c r="K69" t="s">
-        <v>346</v>
+      <c r="A69" t="s">
+        <v>418</v>
+      </c>
+      <c r="C69" t="s">
+        <v>767</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A69,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG10</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A69,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PF7</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>737</v>
-      </c>
-      <c r="B70" t="s">
-        <v>739</v>
-      </c>
-      <c r="C70" t="s">
-        <v>92</v>
-      </c>
-      <c r="D70" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",D$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",E$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG6</v>
-      </c>
-      <c r="F70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",F$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF10</v>
-      </c>
-      <c r="G70" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",G$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",H$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD11</v>
-      </c>
-      <c r="I70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",I$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD12</v>
-      </c>
-      <c r="J70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",J$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC2</v>
-      </c>
-      <c r="K70" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",K$69),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD13</v>
-      </c>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D71" s="1" t="s">
-        <v>734</v>
+      <c r="D71" t="s">
+        <v>420</v>
       </c>
       <c r="E71" t="s">
-        <v>736</v>
-      </c>
-      <c r="F71" t="s">
-        <v>342</v>
-      </c>
-      <c r="G71" t="s">
-        <v>733</v>
-      </c>
-      <c r="H71" t="s">
-        <v>347</v>
-      </c>
-      <c r="I71" t="s">
-        <v>348</v>
-      </c>
-      <c r="J71" t="s">
-        <v>349</v>
-      </c>
-      <c r="K71" t="s">
-        <v>350</v>
-      </c>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
+        <v>421</v>
+      </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>694</v>
+      </c>
+      <c r="D72" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E72" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>695</v>
+      </c>
+      <c r="C73" t="s">
         <v>738</v>
       </c>
-      <c r="B72" t="s">
-        <v>739</v>
-      </c>
-      <c r="C72" t="s">
-        <v>740</v>
-      </c>
-      <c r="D72" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG12</v>
-      </c>
-      <c r="F72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",F$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF4</v>
-      </c>
-      <c r="G72" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",G$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",H$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD4</v>
-      </c>
-      <c r="I72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",I$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH3</v>
-      </c>
-      <c r="J72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",J$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC3</v>
-      </c>
-      <c r="K72" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT("OCTOSPIM_",K$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE10</v>
-      </c>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
+      <c r="D73" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH5</v>
+      </c>
+      <c r="E73" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH4</v>
+      </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>419</v>
       </c>
       <c r="C74" t="s">
-        <v>237</v>
-      </c>
-      <c r="D74" t="str" cm="1">
-        <f t="array" ref="D74" xml:space="preserve"> IF(C74&lt;&gt;"",
-   IFERROR(
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C74))=C74, 0)),
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C74))=C74, 0))
-),"")</f>
-        <v>PE0</v>
+        <v>771</v>
+      </c>
+      <c r="D74" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH8</v>
+      </c>
+      <c r="E74" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH7</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C75" t="s">
-        <v>238</v>
-      </c>
-      <c r="D75" t="str" cm="1">
-        <f t="array" ref="D75" xml:space="preserve"> IF(C75&lt;&gt;"",
-   IFERROR(
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C75))=C75, 0)),
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C75))=C75, 0))
-),"")</f>
-        <v>PE1</v>
+        <v>422</v>
+      </c>
+      <c r="D75" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A75,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E75" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A75,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" t="s">
-        <v>239</v>
-      </c>
-      <c r="D76" t="str" cm="1">
-        <f t="array" ref="D76" xml:space="preserve"> IF(C76&lt;&gt;"",
-   IFERROR(
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C76))=C76, 0)),
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C76))=C76, 0))
-),"")</f>
-        <v>PE2</v>
-      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" t="s">
-        <v>240</v>
-      </c>
-      <c r="D77" t="str" cm="1">
-        <f t="array" ref="D77" xml:space="preserve"> IF(C77&lt;&gt;"",
-   IFERROR(
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C77))=C77, 0)),
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C77))=C77, 0))
-),"")</f>
-        <v>PE3</v>
-      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>689</v>
+        <v>35</v>
+      </c>
+      <c r="C78" t="s">
+        <v>237</v>
       </c>
       <c r="D78" t="str" cm="1">
         <f t="array" ref="D78" xml:space="preserve"> IF(C78&lt;&gt;"",
@@ -5819,15 +5863,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C78))=C78, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C78))=C78, 0))
 ),"")</f>
-        <v>PG4</v>
+        <v>PE0</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>371</v>
+        <v>36</v>
       </c>
       <c r="C79" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D79" t="str" cm="1">
         <f t="array" ref="D79" xml:space="preserve"> IF(C79&lt;&gt;"",
@@ -5835,15 +5879,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C79))=C79, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C79))=C79, 0))
 ),"")</f>
-        <v>PD5</v>
+        <v>PE1</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>372</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="D80" t="str" cm="1">
         <f t="array" ref="D80" xml:space="preserve"> IF(C80&lt;&gt;"",
@@ -5851,15 +5895,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C80))=C80, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C80))=C80, 0))
 ),"")</f>
-        <v>PD6</v>
+        <v>PE2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>373</v>
+        <v>30</v>
       </c>
       <c r="C81" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D81" t="str" cm="1">
         <f t="array" ref="D81" xml:space="preserve"> IF(C81&lt;&gt;"",
@@ -5867,15 +5911,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C81))=C81, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C81))=C81, 0))
 ),"")</f>
-        <v>PE7</v>
+        <v>PE3</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>374</v>
-      </c>
-      <c r="C82" t="s">
-        <v>245</v>
+        <v>43</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>689</v>
       </c>
       <c r="D82" t="str" cm="1">
         <f t="array" ref="D82" xml:space="preserve"> IF(C82&lt;&gt;"",
@@ -5883,15 +5927,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C82))=C82, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C82))=C82, 0))
 ),"")</f>
-        <v>PE8</v>
+        <v>PG4</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>371</v>
       </c>
       <c r="C83" t="s">
-        <v>415</v>
+        <v>223</v>
       </c>
       <c r="D83" t="str" cm="1">
         <f t="array" ref="D83" xml:space="preserve"> IF(C83&lt;&gt;"",
@@ -5899,26 +5943,31 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C83))=C83, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C83))=C83, 0))
 ),"")</f>
-        <v>PH9</v>
+        <v>PD5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>97</v>
-      </c>
-      <c r="C84" s="1"/>
+        <v>372</v>
+      </c>
+      <c r="C84" t="s">
+        <v>225</v>
+      </c>
       <c r="D84" t="str" cm="1">
         <f t="array" ref="D84" xml:space="preserve"> IF(C84&lt;&gt;"",
    IFERROR(
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C84))=C84, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C84))=C84, 0))
 ),"")</f>
-        <v/>
+        <v>PD6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>375</v>
+        <v>373</v>
+      </c>
+      <c r="C85" t="s">
+        <v>244</v>
       </c>
       <c r="D85" t="str" cm="1">
         <f t="array" ref="D85" xml:space="preserve"> IF(C85&lt;&gt;"",
@@ -5926,12 +5975,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C85))=C85, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C85))=C85, 0))
 ),"")</f>
-        <v/>
+        <v>PE7</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>376</v>
+        <v>374</v>
+      </c>
+      <c r="C86" t="s">
+        <v>245</v>
       </c>
       <c r="D86" t="str" cm="1">
         <f t="array" ref="D86" xml:space="preserve"> IF(C86&lt;&gt;"",
@@ -5939,15 +5991,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C86))=C86, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C86))=C86, 0))
 ),"")</f>
-        <v/>
+        <v>PE8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>599</v>
+        <v>415</v>
       </c>
       <c r="D87" t="str" cm="1">
         <f t="array" ref="D87" xml:space="preserve"> IF(C87&lt;&gt;"",
@@ -5955,31 +6007,26 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C87))=C87, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C87))=C87, 0))
 ),"")</f>
-        <v>PC13</v>
+        <v>PH9</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>377</v>
-      </c>
-      <c r="C88" t="s">
-        <v>692</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C88" s="1"/>
       <c r="D88" t="str" cm="1">
         <f t="array" ref="D88" xml:space="preserve"> IF(C88&lt;&gt;"",
    IFERROR(
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C88))=C88, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C88))=C88, 0))
 ),"")</f>
-        <v>PC14-OSC32_IN</v>
+        <v/>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>99</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>701</v>
+        <v>375</v>
       </c>
       <c r="D89" t="str" cm="1">
         <f t="array" ref="D89" xml:space="preserve"> IF(C89&lt;&gt;"",
@@ -5987,56 +6034,83 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C89))=C89, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C89))=C89, 0))
 ),"")</f>
-        <v>PC15-OSC32_OUT</v>
+        <v/>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="str" cm="1">
-        <f t="array" ref="A90">_xlfn.TEXTJOIN(",",TRUE,_xlfn._xlws.FILTER(A74:A89,D74:D89&lt;&gt;""))</f>
-        <v>EXTI0,EXTI1,EXTI2,EXTI3,EXTI4,EXTI5,EXTI6,EXTI7,EXTI8,EXTI9,EXTI13,EXTI14,EXTI15</v>
-      </c>
-      <c r="B90" t="str" cm="1">
-        <f t="array" ref="B90">_xlfn.TEXTJOIN(",", TRUE, --RIGHT(_xlfn.TEXTSPLIT(A90, ","), LEN(_xlfn.TEXTSPLIT(A90, ",")) - 4))</f>
-        <v>0,1,2,3,4,5,6,7,8,9,13,14,15</v>
+      <c r="A90" t="s">
+        <v>376</v>
+      </c>
+      <c r="D90" t="str" cm="1">
+        <f t="array" ref="D90" xml:space="preserve"> IF(C90&lt;&gt;"",
+   IFERROR(
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C90))=C90, 0)),
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C90))=C90, 0))
+),"")</f>
+        <v/>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="1"/>
+      <c r="A91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91" t="s">
+        <v>599</v>
+      </c>
+      <c r="D91" t="str" cm="1">
+        <f t="array" ref="D91" xml:space="preserve"> IF(C91&lt;&gt;"",
+   IFERROR(
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C91))=C91, 0)),
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C91))=C91, 0))
+),"")</f>
+        <v>PC13</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>103</v>
-      </c>
-      <c r="D92" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A92,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH15</v>
+        <v>377</v>
+      </c>
+      <c r="C92" t="s">
+        <v>692</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" ref="D92" xml:space="preserve"> IF(C92&lt;&gt;"",
+   IFERROR(
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C92))=C92, 0)),
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C92))=C92, 0))
+),"")</f>
+        <v>PC14-OSC32_IN</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>351</v>
-      </c>
-      <c r="D93" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A93,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE15</v>
+        <v>99</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" ref="D93" xml:space="preserve"> IF(C93&lt;&gt;"",
+   IFERROR(
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C93))=C93, 0)),
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C93))=C93, 0))
+),"")</f>
+        <v>PC15-OSC32_OUT</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>768</v>
-      </c>
-      <c r="D94" s="1" t="e">
-        <f>_xlfn.XLOOKUP($A94,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+      <c r="A94" t="str" cm="1">
+        <f t="array" ref="A94">_xlfn.TEXTJOIN(",",TRUE,_xlfn._xlws.FILTER(A78:A93,D78:D93&lt;&gt;""))</f>
+        <v>EXTI0,EXTI1,EXTI2,EXTI3,EXTI4,EXTI5,EXTI6,EXTI7,EXTI8,EXTI9,EXTI13,EXTI14,EXTI15</v>
+      </c>
+      <c r="B94" t="str" cm="1">
+        <f t="array" ref="B94">_xlfn.TEXTJOIN(",", TRUE, --RIGHT(_xlfn.TEXTSPLIT(A94, ","), LEN(_xlfn.TEXTSPLIT(A94, ",")) - 4))</f>
+        <v>0,1,2,3,4,5,6,7,8,9,13,14,15</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>769</v>
-      </c>
-      <c r="D95" s="1" t="e">
-        <f>_xlfn.XLOOKUP($A95,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+      <c r="C95" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -6044,293 +6118,341 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
-      </c>
-      <c r="C97" t="s">
-        <v>597</v>
-      </c>
-      <c r="D97" s="1" t="str">
+        <v>103</v>
+      </c>
+      <c r="D97" s="1" t="e">
         <f>_xlfn.XLOOKUP($A97,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA0_C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>353</v>
-      </c>
-      <c r="C98" t="s">
-        <v>596</v>
-      </c>
-      <c r="D98" s="1" t="str">
+        <v>351</v>
+      </c>
+      <c r="D98" s="1" t="e">
         <f>_xlfn.XLOOKUP($A98,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA1_C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>352</v>
-      </c>
-      <c r="C99" t="s">
-        <v>132</v>
-      </c>
-      <c r="D99" s="1" t="str">
+        <v>763</v>
+      </c>
+      <c r="D99" s="1" t="e">
         <f>_xlfn.XLOOKUP($A99,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC2_C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>354</v>
-      </c>
-      <c r="C100" t="s">
-        <v>133</v>
-      </c>
-      <c r="D100" s="1" t="str">
+        <v>764</v>
+      </c>
+      <c r="D100" s="1" t="e">
         <f>_xlfn.XLOOKUP($A100,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC3_C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>714</v>
-      </c>
-      <c r="C101" t="s">
-        <v>767</v>
-      </c>
-      <c r="D101" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A101,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC0</v>
-      </c>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>712</v>
+        <v>106</v>
       </c>
       <c r="C102" t="s">
-        <v>767</v>
+        <v>597</v>
       </c>
       <c r="D102" s="1" t="str">
         <f>_xlfn.XLOOKUP($A102,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH2</v>
+        <v>PA0_C</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>353</v>
+      </c>
+      <c r="C103" t="s">
+        <v>596</v>
+      </c>
+      <c r="D103" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A103,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA1_C</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>715</v>
+        <v>352</v>
+      </c>
+      <c r="C104" t="s">
+        <v>132</v>
       </c>
       <c r="D104" s="1" t="str">
         <f>_xlfn.XLOOKUP($A104,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PB8</v>
+        <v>PC2_C</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>716</v>
+        <v>354</v>
+      </c>
+      <c r="C105" t="s">
+        <v>133</v>
       </c>
       <c r="D105" s="1" t="str">
         <f>_xlfn.XLOOKUP($A105,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PB9</v>
+        <v>PC3_C</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>717</v>
-      </c>
-      <c r="D106" s="1" t="e">
+        <v>713</v>
+      </c>
+      <c r="C106" t="s">
+        <v>771</v>
+      </c>
+      <c r="D106" s="1" t="str">
         <f>_xlfn.XLOOKUP($A106,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+        <v>PC0</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>718</v>
-      </c>
-      <c r="D107" s="1" t="e">
+        <v>711</v>
+      </c>
+      <c r="C107" t="s">
+        <v>771</v>
+      </c>
+      <c r="D107" s="1" t="str">
         <f>_xlfn.XLOOKUP($A107,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>720</v>
-      </c>
-      <c r="D108" s="1" t="e">
-        <f>_xlfn.XLOOKUP($A108,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+        <v>PH2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>719</v>
-      </c>
-      <c r="D109" s="1" t="e">
+        <v>714</v>
+      </c>
+      <c r="C109" t="s">
+        <v>771</v>
+      </c>
+      <c r="D109" s="1" t="str">
         <f>_xlfn.XLOOKUP($A109,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+        <v>PB8</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>721</v>
-      </c>
-      <c r="D110" s="1" t="e">
+        <v>715</v>
+      </c>
+      <c r="C110" t="s">
+        <v>771</v>
+      </c>
+      <c r="D110" s="1" t="str">
         <f>_xlfn.XLOOKUP($A110,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+        <v>PB9</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="D111" s="1" t="e">
         <f>_xlfn.XLOOKUP($A111,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
     </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>717</v>
+      </c>
+      <c r="D112" s="1" t="e">
+        <f>_xlfn.XLOOKUP($A112,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>692</v>
-      </c>
-      <c r="C113" t="s">
-        <v>732</v>
-      </c>
-      <c r="D113" s="1" t="str">
+        <v>719</v>
+      </c>
+      <c r="D113" s="1" t="e">
         <f>_xlfn.XLOOKUP($A113,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC14-OSC32_IN</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>693</v>
-      </c>
-      <c r="D114" s="1" t="str">
+        <v>718</v>
+      </c>
+      <c r="D114" s="1" t="e">
         <f>_xlfn.XLOOKUP($A114,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF15</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D115" s="1"/>
+      <c r="A115" t="s">
+        <v>720</v>
+      </c>
+      <c r="D115" s="1" t="e">
+        <f>_xlfn.XLOOKUP($A115,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>355</v>
-      </c>
-      <c r="E116" t="s">
-        <v>356</v>
-      </c>
-      <c r="F116" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>358</v>
-      </c>
-      <c r="D117" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A117,"_",D$116),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA11</v>
-      </c>
-      <c r="E117" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A117,"_",E$116),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA12</v>
-      </c>
-      <c r="F117" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A117,"_",F$116),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="A116" t="s">
+        <v>721</v>
+      </c>
+      <c r="D116" s="1" t="e">
+        <f>_xlfn.XLOOKUP($A116,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>692</v>
+      </c>
+      <c r="C118" t="s">
+        <v>731</v>
+      </c>
+      <c r="D118" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A118,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC14-OSC32_IN</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>723</v>
-      </c>
-      <c r="C119" t="s">
-        <v>583</v>
+        <v>693</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A119,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PF15</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>723</v>
-      </c>
-      <c r="C120" t="s">
-        <v>584</v>
-      </c>
+      <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>723</v>
-      </c>
-      <c r="C121" t="s">
-        <v>585</v>
+      <c r="D121" t="s">
+        <v>355</v>
+      </c>
+      <c r="E121" t="s">
+        <v>356</v>
+      </c>
+      <c r="F121" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>723</v>
+        <v>358</v>
       </c>
       <c r="C122" t="s">
-        <v>586</v>
+        <v>772</v>
+      </c>
+      <c r="D122" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",D$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA11</v>
+      </c>
+      <c r="E122" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",E$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA12</v>
+      </c>
+      <c r="F122" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",F$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C124" t="s">
-        <v>127</v>
+        <v>583</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C125" t="s">
-        <v>128</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C126" t="s">
-        <v>129</v>
+        <v>585</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="C127" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>728</v>
-      </c>
-      <c r="C128" t="s">
-        <v>130</v>
+        <v>586</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C129" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C130" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C131" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>726</v>
+      </c>
+      <c r="C132" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>727</v>
+      </c>
+      <c r="C133" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>728</v>
+      </c>
+      <c r="C134" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>729</v>
+      </c>
+      <c r="C135" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>730</v>
+      </c>
+      <c r="C136" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6415,7 +6537,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6442,7 +6564,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6498,7 +6620,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6525,7 +6647,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6552,7 +6674,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6560,7 +6682,7 @@
         <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>138</v>
@@ -6579,7 +6701,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6606,7 +6728,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6633,7 +6755,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6660,7 +6782,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6687,7 +6809,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -6714,7 +6836,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6741,7 +6863,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -6768,7 +6890,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -6795,7 +6917,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -6822,7 +6944,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6849,7 +6971,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -6905,7 +7027,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6932,7 +7054,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -6959,7 +7081,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6986,7 +7108,7 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6994,7 +7116,7 @@
         <v>183</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>138</v>
@@ -7013,7 +7135,7 @@
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -7040,7 +7162,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -7067,7 +7189,7 @@
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -7094,7 +7216,7 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -7102,7 +7224,7 @@
         <v>305</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>138</v>
@@ -7120,7 +7242,7 @@
         <v>189</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>1</v>
@@ -7149,7 +7271,7 @@
         <v>189</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>1</v>
@@ -7179,7 +7301,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -7206,7 +7328,7 @@
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -7233,7 +7355,7 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -7260,7 +7382,7 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -7287,7 +7409,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -7314,7 +7436,7 @@
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -7322,7 +7444,7 @@
         <v>93</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>138</v>
@@ -7340,7 +7462,7 @@
         <v>138</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -7370,7 +7492,7 @@
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -7397,7 +7519,7 @@
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -7434,7 +7556,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>138</v>
@@ -7453,7 +7575,7 @@
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -7509,7 +7631,7 @@
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -7536,7 +7658,7 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -7563,7 +7685,7 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -7590,7 +7712,7 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -7617,7 +7739,7 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -7644,7 +7766,7 @@
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -7671,7 +7793,7 @@
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -7698,7 +7820,7 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -7725,7 +7847,7 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -7786,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>149</v>
       </c>
@@ -7809,7 +7931,7 @@
         <v>138</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>701</v>
+        <v>785</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>1</v>
@@ -7820,7 +7942,7 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>138</v>
@@ -7839,7 +7961,7 @@
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -7847,7 +7969,7 @@
         <v>32</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>138</v>
@@ -7866,7 +7988,7 @@
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -7893,7 +8015,7 @@
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -7920,7 +8042,7 @@
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -7928,7 +8050,7 @@
         <v>221</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>138</v>
@@ -7947,7 +8069,7 @@
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -7974,7 +8096,7 @@
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -8001,7 +8123,7 @@
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -8009,7 +8131,7 @@
         <v>104</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>138</v>
@@ -8028,7 +8150,7 @@
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -8055,7 +8177,7 @@
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -8082,7 +8204,7 @@
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -8108,7 +8230,7 @@
         <v>138</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="I64" s="1" t="b">
         <v>1</v>
@@ -8138,7 +8260,7 @@
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -8165,7 +8287,7 @@
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -8192,7 +8314,7 @@
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -8219,7 +8341,7 @@
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -8246,7 +8368,7 @@
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -8273,7 +8395,7 @@
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -8300,7 +8422,7 @@
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -8327,7 +8449,7 @@
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -8354,7 +8476,7 @@
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -8381,7 +8503,7 @@
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -8408,7 +8530,7 @@
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -8435,7 +8557,7 @@
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -8462,7 +8584,7 @@
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -8489,7 +8611,7 @@
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -8516,7 +8638,7 @@
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -8524,7 +8646,7 @@
         <v>247</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>138</v>
@@ -8543,7 +8665,7 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -8570,7 +8692,7 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -8597,7 +8719,7 @@
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -8624,7 +8746,7 @@
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -8651,7 +8773,7 @@
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -8662,22 +8784,22 @@
         <v>138</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>141</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>138</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>351</v>
+        <v>779</v>
       </c>
       <c r="I85" s="1" t="b">
         <v>1</v>
@@ -8707,7 +8829,7 @@
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -8734,7 +8856,7 @@
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -8761,7 +8883,7 @@
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -8788,7 +8910,7 @@
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -8796,7 +8918,7 @@
         <v>260</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>138</v>
@@ -8815,7 +8937,7 @@
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -8841,7 +8963,7 @@
         <v>138</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="I91" s="1" t="b">
         <v>1</v>
@@ -8871,7 +8993,7 @@
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -8898,7 +9020,7 @@
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -8925,7 +9047,7 @@
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -8952,7 +9074,7 @@
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -8979,7 +9101,7 @@
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -9006,7 +9128,7 @@
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -9033,7 +9155,7 @@
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -9060,7 +9182,7 @@
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -9087,7 +9209,7 @@
       </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -9143,7 +9265,7 @@
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -9170,7 +9292,7 @@
       </c>
       <c r="H103" s="1"/>
       <c r="I103" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -9265,7 +9387,7 @@
         <v>118</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>138</v>
@@ -9284,7 +9406,7 @@
       </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -9311,7 +9433,7 @@
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -9348,7 +9470,7 @@
         <v>121</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>138</v>
@@ -9367,7 +9489,7 @@
       </c>
       <c r="H110" s="1"/>
       <c r="I110" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -9375,7 +9497,7 @@
         <v>52</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>138</v>
@@ -9394,7 +9516,7 @@
       </c>
       <c r="H111" s="1"/>
       <c r="I111" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -9421,7 +9543,7 @@
       </c>
       <c r="H112" s="1"/>
       <c r="I112" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -9448,7 +9570,7 @@
       </c>
       <c r="H113" s="1"/>
       <c r="I113" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -9456,7 +9578,7 @@
         <v>287</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>138</v>
@@ -9475,7 +9597,7 @@
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -9502,7 +9624,7 @@
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -9510,7 +9632,7 @@
         <v>53</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>138</v>
@@ -9529,7 +9651,7 @@
       </c>
       <c r="H116" s="1"/>
       <c r="I116" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -9585,7 +9707,7 @@
       </c>
       <c r="H118" s="1"/>
       <c r="I118" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -9612,7 +9734,7 @@
       </c>
       <c r="H119" s="1"/>
       <c r="I119" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -9620,7 +9742,7 @@
         <v>123</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>138</v>
@@ -9638,7 +9760,7 @@
         <v>138</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I120" s="1" t="b">
         <v>1</v>
@@ -9649,7 +9771,7 @@
         <v>291</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>138</v>
@@ -9668,7 +9790,7 @@
       </c>
       <c r="H121" s="1"/>
       <c r="I121" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -9676,7 +9798,7 @@
         <v>124</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>138</v>
@@ -9695,7 +9817,7 @@
       </c>
       <c r="H122" s="1"/>
       <c r="I122" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -9703,7 +9825,7 @@
         <v>292</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>138</v>
@@ -9722,7 +9844,7 @@
       </c>
       <c r="H123" s="1"/>
       <c r="I123" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -9749,7 +9871,7 @@
       </c>
       <c r="H124" s="1"/>
       <c r="I124" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -9776,7 +9898,7 @@
       </c>
       <c r="H125" s="1"/>
       <c r="I125" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -9803,7 +9925,7 @@
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -9811,7 +9933,7 @@
         <v>95</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>138</v>
@@ -9859,7 +9981,7 @@
       </c>
       <c r="H128" s="1"/>
       <c r="I128" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -9886,7 +10008,7 @@
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -9913,7 +10035,7 @@
       </c>
       <c r="H130" s="1"/>
       <c r="I130" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -9940,7 +10062,7 @@
       </c>
       <c r="H131" s="1"/>
       <c r="I131" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -9967,7 +10089,7 @@
       </c>
       <c r="H132" s="1"/>
       <c r="I132" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -9978,22 +10100,22 @@
         <v>138</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>141</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>138</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>103</v>
+        <v>778</v>
       </c>
       <c r="I133" s="1" t="b">
         <v>1</v>
@@ -10611,7 +10733,7 @@
         <v>92</v>
       </c>
       <c r="G35" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="J35" t="s">
         <v>546</v>
@@ -10850,7 +10972,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
@@ -14516,7 +14638,7 @@
         <v>ETH_ACT_LED</v>
       </c>
       <c r="C155" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -14528,7 +14650,7 @@
         <v>ETH_LINK_LED</v>
       </c>
       <c r="C156" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FPGA, FLASH and INT updates.
</commit_message>
<xml_diff>
--- a/Design/port peripheral mapping.xlsx
+++ b/Design/port peripheral mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hydra\Documents\DipTrace\Projects\MakerPnPControl\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A384E11-6865-4347-87E1-ACBFFA2EC4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B32A29-7731-490D-A4BB-9AE2EC204810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="3990" windowWidth="29775" windowHeight="20505" xr2:uid="{C3A3646F-069D-4AE0-AC21-8ACD43A56D36}"/>
+    <workbookView xWindow="17715" yWindow="15375" windowWidth="19725" windowHeight="12420" activeTab="2" xr2:uid="{C3A3646F-069D-4AE0-AC21-8ACD43A56D36}"/>
   </bookViews>
   <sheets>
     <sheet name="UFBGA176+25 Ports" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PORT_PINS!$A$11:$I$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'UFBGA176+25 GPIOs'!$A$1:$I$133</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'UFBFA176+25 Peripherals'!$A$1:$O$122</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'UFBFA176+25 Peripherals'!$A$1:$O$121</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'UFBGA176+25 GPIOs'!$A$1:$H$133</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="794">
   <si>
     <t>Port</t>
   </si>
@@ -2395,9 +2395,6 @@
     <t>Devices on expansion port can trigger MCU action since the FPGA is an IO expander</t>
   </si>
   <si>
-    <t>EXTI15_FPGA_RESERVED_OCTOSPI2_NCS_4</t>
-  </si>
-  <si>
     <t>^ NOTE: all OCTOSPI_NCS_x pins are on EXTI15 pin Px15 so use here is flexible</t>
   </si>
   <si>
@@ -2444,6 +2441,15 @@
   </si>
   <si>
     <t>Interrupt signal</t>
+  </si>
+  <si>
+    <t>EXTI15_FPGA_INT</t>
+  </si>
+  <si>
+    <t>EXTI14_FPGA_INT</t>
+  </si>
+  <si>
+    <t>EXTI15_FPGA_CDONE</t>
   </si>
 </sst>
 </file>
@@ -2888,7 +2894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5E5D7C-73CD-4684-9992-8F63AACE455E}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -3163,9 +3169,9 @@
       <c r="A9" t="s">
         <v>680</v>
       </c>
-      <c r="C9" t="str">
-        <f>'UFBFA176+25 Peripherals'!B94</f>
-        <v>0,1,2,3,4,5,6,7,8,9,13,14,15</v>
+      <c r="C9" t="e">
+        <f>'UFBFA176+25 Peripherals'!B93</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3333,10 +3339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB4DCCF-6249-4668-B225-7F06A2FCE957}">
-  <dimension ref="A1:P136"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5168,51 +5174,88 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>775</v>
       </c>
-      <c r="B52" t="s">
-        <v>772</v>
-      </c>
-      <c r="C52" t="s">
-        <v>92</v>
-      </c>
-      <c r="D52" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A52,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC15-OSC32_OUT</v>
-      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>776</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="D53" t="s">
+        <v>318</v>
+      </c>
+      <c r="E53" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>318</v>
-      </c>
-      <c r="E54" t="s">
-        <v>319</v>
+      <c r="A54" t="s">
+        <v>320</v>
+      </c>
+      <c r="C54" t="s">
+        <v>321</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A54,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA10</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A54,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA9</v>
+      </c>
+      <c r="H54" t="str" cm="1">
+        <f t="array" ref="H54">_xlfn.LET(
+    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D54:G54),
+    _xlpm.cleaned,
+        _xlfn.TEXTJOIN("", TRUE,
+            IF(
+                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
+                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
+                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
+                ""
+            )
+        ),
+    IFERROR(
+        _xlfn.TEXTJOIN(",", TRUE,
+            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
+        ),
+        ""
+    )
+)</f>
+        <v>10,9</v>
+      </c>
+      <c r="I54" t="str" cm="1">
+        <f t="array" ref="I54">IF(
+    H54="",
+    "",
+    _xlfn.TEXTJOIN(
+        ",",
+        TRUE,
+        _xlfn.SORTBY(
+            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")))),
+            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H54, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H54, ","))))
+        )
+    )
+)</f>
+        <v>9,10</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>320</v>
+        <v>86</v>
       </c>
       <c r="C55" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA10</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD6</v>
       </c>
       <c r="E55" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA9</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A55,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD5</v>
       </c>
       <c r="H55" t="str" cm="1">
         <f t="array" ref="H55">_xlfn.LET(
@@ -5233,7 +5276,7 @@
         ""
     )
 )</f>
-        <v>10,9</v>
+        <v>6,5</v>
       </c>
       <c r="I55" t="str" cm="1">
         <f t="array" ref="I55">IF(
@@ -5248,23 +5291,23 @@
         )
     )
 )</f>
-        <v>9,10</v>
+        <v>5,6</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD6</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD9</v>
       </c>
       <c r="E56" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD5</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A56,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD8</v>
       </c>
       <c r="H56" t="str" cm="1">
         <f t="array" ref="H56">_xlfn.LET(
@@ -5285,7 +5328,7 @@
         ""
     )
 )</f>
-        <v>6,5</v>
+        <v>9,8</v>
       </c>
       <c r="I56" t="str" cm="1">
         <f t="array" ref="I56">IF(
@@ -5300,23 +5343,23 @@
         )
     )
 )</f>
-        <v>5,6</v>
+        <v>8,9</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>323</v>
+        <v>756</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD9</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD0</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD8</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A57,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD1</v>
       </c>
       <c r="H57" t="str" cm="1">
         <f t="array" ref="H57">_xlfn.LET(
@@ -5337,7 +5380,7 @@
         ""
     )
 )</f>
-        <v>9,8</v>
+        <v>0,1</v>
       </c>
       <c r="I57" t="str" cm="1">
         <f t="array" ref="I57">IF(
@@ -5352,23 +5395,23 @@
         )
     )
 )</f>
-        <v>8,9</v>
+        <v>0,1</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>756</v>
+        <v>324</v>
       </c>
       <c r="D58" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD0</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PD2</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD1</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A58,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PC12</v>
       </c>
       <c r="H58" t="str" cm="1">
         <f t="array" ref="H58">_xlfn.LET(
@@ -5389,7 +5432,7 @@
         ""
     )
 )</f>
-        <v>0,1</v>
+        <v>2,12</v>
       </c>
       <c r="I58" t="str" cm="1">
         <f t="array" ref="I58">IF(
@@ -5404,23 +5447,23 @@
         )
     )
 )</f>
-        <v>0,1</v>
+        <v>2,12</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>324</v>
+        <v>761</v>
       </c>
       <c r="D59" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PD2</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG9</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC12</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A59,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG14</v>
       </c>
       <c r="H59" t="str" cm="1">
         <f t="array" ref="H59">_xlfn.LET(
@@ -5441,7 +5484,7 @@
         ""
     )
 )</f>
-        <v>2,12</v>
+        <v>9,14</v>
       </c>
       <c r="I59" t="str" cm="1">
         <f t="array" ref="I59">IF(
@@ -5456,23 +5499,23 @@
         )
     )
 )</f>
-        <v>2,12</v>
+        <v>9,14</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>761</v>
+        <v>326</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG9</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE7</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG14</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A60,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE8</v>
       </c>
       <c r="H60" t="str" cm="1">
         <f t="array" ref="H60">_xlfn.LET(
@@ -5493,7 +5536,7 @@
         ""
     )
 )</f>
-        <v>9,14</v>
+        <v>7,8</v>
       </c>
       <c r="I60" t="str" cm="1">
         <f t="array" ref="I60">IF(
@@ -5508,23 +5551,23 @@
         )
     )
 )</f>
-        <v>9,14</v>
+        <v>7,8</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C61" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE7</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE0</v>
       </c>
       <c r="E61" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE8</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A61,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE1</v>
       </c>
       <c r="H61" t="str" cm="1">
         <f t="array" ref="H61">_xlfn.LET(
@@ -5545,7 +5588,7 @@
         ""
     )
 )</f>
-        <v>7,8</v>
+        <v>0,1</v>
       </c>
       <c r="I61" t="str" cm="1">
         <f t="array" ref="I61">IF(
@@ -5560,23 +5603,23 @@
         )
     )
 )</f>
-        <v>7,8</v>
+        <v>0,1</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D62" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE0</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG0</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE1</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A62,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG1</v>
       </c>
       <c r="H62" t="str" cm="1">
         <f t="array" ref="H62">_xlfn.LET(
@@ -5617,18 +5660,18 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>325</v>
+        <v>378</v>
       </c>
       <c r="D63" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG0</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",D$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE2</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG1</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A63,"_",E$53),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PE3</v>
       </c>
       <c r="H63" t="str" cm="1">
         <f t="array" ref="H63">_xlfn.LET(
@@ -5649,7 +5692,7 @@
         ""
     )
 )</f>
-        <v>0,1</v>
+        <v>2,3</v>
       </c>
       <c r="I63" t="str" cm="1">
         <f t="array" ref="I63">IF(
@@ -5664,213 +5707,177 @@
         )
     )
 )</f>
-        <v>0,1</v>
+        <v>2,3</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" t="s">
-        <v>378</v>
-      </c>
-      <c r="D64" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",D$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE2</v>
-      </c>
-      <c r="E64" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A64,"_",E$54),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PE3</v>
-      </c>
-      <c r="H64" t="str" cm="1">
-        <f t="array" ref="H64">_xlfn.LET(
-    _xlpm.joined, _xlfn.TEXTJOIN(",", TRUE, D64:G64),
-    _xlpm.cleaned,
-        _xlfn.TEXTJOIN("", TRUE,
-            IF(
-                (ISNUMBER(--MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1))) +
-                (MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1) = ","),
-                MID(_xlpm.joined, _xlfn.SEQUENCE(LEN(_xlpm.joined)), 1),
-                ""
-            )
-        ),
-    IFERROR(
-        _xlfn.TEXTJOIN(",", TRUE,
-            _xlfn._xlws.FILTER(_xlfn.TEXTSPLIT(_xlpm.cleaned, ","), _xlfn.TEXTSPLIT(_xlpm.cleaned, ",")&lt;&gt;"")
-        ),
-        ""
-    )
-)</f>
-        <v>2,3</v>
-      </c>
-      <c r="I64" t="str" cm="1">
-        <f t="array" ref="I64">IF(
-    H64="",
-    "",
-    _xlfn.TEXTJOIN(
-        ",",
-        TRUE,
-        _xlfn.SORTBY(
-            _xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")))),
-            --_xlfn._xlws.FILTER(--TRIM(_xlfn.TEXTSPLIT(H64, ",")), ISNUMBER(--TRIM(_xlfn.TEXTSPLIT(H64, ","))))
-        )
-    )
-)</f>
-        <v>2,3</v>
-      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="D65" t="s">
+        <v>318</v>
+      </c>
+      <c r="E65" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>318</v>
-      </c>
-      <c r="E66" t="s">
-        <v>319</v>
+      <c r="A66" t="s">
+        <v>414</v>
+      </c>
+      <c r="C66" t="s">
+        <v>758</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A66,"_",D$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH14</v>
+      </c>
+      <c r="E66" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A66,"_",E$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH13</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>414</v>
-      </c>
-      <c r="C67" t="s">
-        <v>758</v>
-      </c>
-      <c r="D67" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH14</v>
-      </c>
-      <c r="E67" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH13</v>
+        <v>415</v>
+      </c>
+      <c r="D67" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",D$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E67" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A67,"_",E$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>415</v>
-      </c>
-      <c r="D68" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>416</v>
+      </c>
+      <c r="C68" t="s">
+        <v>757</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",D$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PG10</v>
+      </c>
+      <c r="E68" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",E$65),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PF7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>418</v>
+      </c>
+      <c r="E70" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>684</v>
+      </c>
+      <c r="D71" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A71,"_",D$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
-      <c r="E68" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A68,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="E71" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A71,"_",E$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>416</v>
-      </c>
-      <c r="C69" t="s">
-        <v>757</v>
-      </c>
-      <c r="D69" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A69,"_",D$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PG10</v>
-      </c>
-      <c r="E69" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A69,"_",E$66),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>418</v>
-      </c>
-      <c r="E71" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>684</v>
-      </c>
-      <c r="D72" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E72" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
+        <v>685</v>
+      </c>
+      <c r="C72" t="s">
+        <v>728</v>
+      </c>
+      <c r="D72" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",D$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH5</v>
+      </c>
+      <c r="E72" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A72,"_",E$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH4</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>685</v>
+        <v>417</v>
       </c>
       <c r="C73" t="s">
-        <v>728</v>
+        <v>761</v>
       </c>
       <c r="D73" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH5</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",D$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH8</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH4</v>
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A73,"_",E$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PH7</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>417</v>
-      </c>
-      <c r="C74" t="s">
-        <v>761</v>
-      </c>
-      <c r="D74" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH8</v>
-      </c>
-      <c r="E74" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PH7</v>
+        <v>420</v>
+      </c>
+      <c r="D74" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",D$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E74" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A74,"_",E$70),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>420</v>
-      </c>
-      <c r="D75" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A75,"_",D$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E75" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A75,"_",E$71),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
+      <c r="A77" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" t="str" cm="1">
+        <f t="array" ref="D77" xml:space="preserve"> IF(C77&lt;&gt;"",
+   IFERROR(
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C77))=C77, 0)),
+      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C77))=C77, 0))
+),"")</f>
+        <v>PE0</v>
+      </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C78" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D78" t="str" cm="1">
         <f t="array" ref="D78" xml:space="preserve"> IF(C78&lt;&gt;"",
@@ -5878,15 +5885,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C78))=C78, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C78))=C78, 0))
 ),"")</f>
-        <v>PE0</v>
+        <v>PE1</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D79" t="str" cm="1">
         <f t="array" ref="D79" xml:space="preserve"> IF(C79&lt;&gt;"",
@@ -5894,15 +5901,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C79))=C79, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C79))=C79, 0))
 ),"")</f>
-        <v>PE1</v>
+        <v>PE2</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D80" t="str" cm="1">
         <f t="array" ref="D80" xml:space="preserve"> IF(C80&lt;&gt;"",
@@ -5910,15 +5917,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C80))=C80, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C80))=C80, 0))
 ),"")</f>
-        <v>PE2</v>
+        <v>PE3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>30</v>
-      </c>
-      <c r="C81" t="s">
-        <v>238</v>
+        <v>43</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>679</v>
       </c>
       <c r="D81" t="str" cm="1">
         <f t="array" ref="D81" xml:space="preserve"> IF(C81&lt;&gt;"",
@@ -5926,15 +5933,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C81))=C81, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C81))=C81, 0))
 ),"")</f>
-        <v>PE3</v>
+        <v>PG4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>43</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>679</v>
+        <v>369</v>
+      </c>
+      <c r="C82" t="s">
+        <v>221</v>
       </c>
       <c r="D82" t="str" cm="1">
         <f t="array" ref="D82" xml:space="preserve"> IF(C82&lt;&gt;"",
@@ -5942,15 +5949,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C82))=C82, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C82))=C82, 0))
 ),"")</f>
-        <v>PG4</v>
+        <v>PD5</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C83" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D83" t="str" cm="1">
         <f t="array" ref="D83" xml:space="preserve"> IF(C83&lt;&gt;"",
@@ -5958,15 +5965,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C83))=C83, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C83))=C83, 0))
 ),"")</f>
-        <v>PD5</v>
+        <v>PD6</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C84" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="D84" t="str" cm="1">
         <f t="array" ref="D84" xml:space="preserve"> IF(C84&lt;&gt;"",
@@ -5974,15 +5981,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C84))=C84, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C84))=C84, 0))
 ),"")</f>
-        <v>PD6</v>
+        <v>PE7</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C85" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D85" t="str" cm="1">
         <f t="array" ref="D85" xml:space="preserve"> IF(C85&lt;&gt;"",
@@ -5990,15 +5997,15 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C85))=C85, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C85))=C85, 0))
 ),"")</f>
-        <v>PE7</v>
+        <v>PE8</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>372</v>
+        <v>94</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>413</v>
       </c>
       <c r="D86" t="str" cm="1">
         <f t="array" ref="D86" xml:space="preserve"> IF(C86&lt;&gt;"",
@@ -6006,30 +6013,27 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C86))=C86, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C86))=C86, 0))
 ),"")</f>
-        <v>PE8</v>
+        <v>PH9</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
-      </c>
-      <c r="C87" t="s">
-        <v>413</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C87" s="1"/>
       <c r="D87" t="str" cm="1">
         <f t="array" ref="D87" xml:space="preserve"> IF(C87&lt;&gt;"",
    IFERROR(
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C87))=C87, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C87))=C87, 0))
 ),"")</f>
-        <v>PH9</v>
+        <v/>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
-      </c>
-      <c r="C88" s="1"/>
+        <v>373</v>
+      </c>
       <c r="D88" t="str" cm="1">
         <f t="array" ref="D88" xml:space="preserve"> IF(C88&lt;&gt;"",
    IFERROR(
@@ -6041,7 +6045,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D89" t="str" cm="1">
         <f t="array" ref="D89" xml:space="preserve"> IF(C89&lt;&gt;"",
@@ -6054,7 +6058,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>374</v>
+        <v>101</v>
+      </c>
+      <c r="C90" t="s">
+        <v>589</v>
       </c>
       <c r="D90" t="str" cm="1">
         <f t="array" ref="D90" xml:space="preserve"> IF(C90&lt;&gt;"",
@@ -6062,78 +6069,71 @@
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C90))=C90, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C90))=C90, 0))
 ),"")</f>
-        <v/>
+        <v>PC13</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>375</v>
       </c>
       <c r="C91" t="s">
-        <v>589</v>
-      </c>
-      <c r="D91" t="str" cm="1">
+        <v>682</v>
+      </c>
+      <c r="D91" t="e" cm="1">
         <f t="array" ref="D91" xml:space="preserve"> IF(C91&lt;&gt;"",
    IFERROR(
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C91))=C91, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C91))=C91, 0))
 ),"")</f>
-        <v>PC13</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>375</v>
-      </c>
-      <c r="C92" t="s">
-        <v>682</v>
-      </c>
-      <c r="D92" t="str" cm="1">
+        <v>99</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D92" t="e" cm="1">
         <f t="array" ref="D92" xml:space="preserve"> IF(C92&lt;&gt;"",
    IFERROR(
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C92))=C92, 0)),
       INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C92))=C92, 0))
 ),"")</f>
-        <v>PC14-OSC32_IN</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>99</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="D93" t="str" cm="1">
-        <f t="array" ref="D93" xml:space="preserve"> IF(C93&lt;&gt;"",
-   IFERROR(
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$H$2:$H$133, LEN(C93))=C93, 0)),
-      INDEX('UFBGA176+25 GPIOs'!$A$2:$A$133, MATCH(TRUE, LEFT('UFBGA176+25 GPIOs'!$B$2:$B$133, LEN(C93))=C93, 0))
-),"")</f>
-        <v>PC15-OSC32_OUT</v>
+      <c r="A93" t="e" cm="1">
+        <f t="array" ref="A93">_xlfn.TEXTJOIN(",",TRUE,_xlfn._xlws.FILTER(A77:A92,D77:D92&lt;&gt;""))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="B93" t="e" cm="1">
+        <f t="array" ref="B93">_xlfn.TEXTJOIN(",", TRUE, --RIGHT(_xlfn.TEXTSPLIT(A93, ","), LEN(_xlfn.TEXTSPLIT(A93, ",")) - 4))</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="str" cm="1">
-        <f t="array" ref="A94">_xlfn.TEXTJOIN(",",TRUE,_xlfn._xlws.FILTER(A78:A93,D78:D93&lt;&gt;""))</f>
-        <v>EXTI0,EXTI1,EXTI2,EXTI3,EXTI4,EXTI5,EXTI6,EXTI7,EXTI8,EXTI9,EXTI13,EXTI14,EXTI15</v>
-      </c>
-      <c r="B94" t="str" cm="1">
-        <f t="array" ref="B94">_xlfn.TEXTJOIN(",", TRUE, --RIGHT(_xlfn.TEXTSPLIT(A94, ","), LEN(_xlfn.TEXTSPLIT(A94, ",")) - 4))</f>
-        <v>0,1,2,3,4,5,6,7,8,9,13,14,15</v>
+      <c r="C94" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>774</v>
-      </c>
+      <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="1"/>
+      <c r="A96" t="s">
+        <v>103</v>
+      </c>
+      <c r="D96" s="1" t="e">
+        <f>_xlfn.XLOOKUP($A96,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>103</v>
+        <v>349</v>
       </c>
       <c r="D97" s="1" t="e">
         <f>_xlfn.XLOOKUP($A97,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6142,7 +6142,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>349</v>
+        <v>753</v>
       </c>
       <c r="D98" s="1" t="e">
         <f>_xlfn.XLOOKUP($A98,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D99" s="1" t="e">
         <f>_xlfn.XLOOKUP($A99,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6159,116 +6159,116 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>754</v>
-      </c>
-      <c r="D100" s="1" t="e">
-        <f>_xlfn.XLOOKUP($A100,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="1"/>
+      <c r="A101" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>783</v>
+      </c>
+      <c r="D101" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A101,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PA0_C</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>351</v>
       </c>
       <c r="C102" t="s">
         <v>784</v>
       </c>
       <c r="D102" s="1" t="str">
         <f>_xlfn.XLOOKUP($A102,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA0_C</v>
+        <v>PA1_C</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C103" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="D103" s="1" t="str">
         <f>_xlfn.XLOOKUP($A103,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PA1_C</v>
+        <v>PC2_C</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C104" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D104" s="1" t="str">
         <f>_xlfn.XLOOKUP($A104,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC2_C</v>
+        <v>PC3_C</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>352</v>
+        <v>703</v>
       </c>
       <c r="C105" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D105" s="1" t="str">
         <f>_xlfn.XLOOKUP($A105,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC3_C</v>
+        <v>PC0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C106" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D106" s="1" t="str">
         <f>_xlfn.XLOOKUP($A106,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>701</v>
-      </c>
-      <c r="C107" t="s">
-        <v>783</v>
-      </c>
-      <c r="D107" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A107,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>PH2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>704</v>
+      </c>
+      <c r="C108" t="s">
+        <v>761</v>
+      </c>
+      <c r="D108" s="1" t="str">
+        <f>_xlfn.XLOOKUP($A108,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+        <v>PB8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C109" t="s">
         <v>761</v>
       </c>
       <c r="D109" s="1" t="str">
         <f>_xlfn.XLOOKUP($A109,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PB8</v>
+        <v>PB9</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>705</v>
-      </c>
-      <c r="C110" t="s">
-        <v>761</v>
-      </c>
-      <c r="D110" s="1" t="str">
+        <v>706</v>
+      </c>
+      <c r="D110" s="1" t="e">
         <f>_xlfn.XLOOKUP($A110,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PB9</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D111" s="1" t="e">
         <f>_xlfn.XLOOKUP($A111,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6277,7 +6277,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D112" s="1" t="e">
         <f>_xlfn.XLOOKUP($A112,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D113" s="1" t="e">
         <f>_xlfn.XLOOKUP($A113,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D114" s="1" t="e">
         <f>_xlfn.XLOOKUP($A114,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
@@ -6304,75 +6304,74 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D115" s="1" t="e">
         <f>_xlfn.XLOOKUP($A115,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>711</v>
-      </c>
-      <c r="D116" s="1" t="e">
-        <f>_xlfn.XLOOKUP($A116,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>682</v>
+      </c>
+      <c r="C117" t="s">
+        <v>721</v>
+      </c>
+      <c r="D117" s="1" t="e">
+        <f>_xlfn.XLOOKUP($A117,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>682</v>
-      </c>
-      <c r="C118" t="s">
-        <v>721</v>
+        <v>683</v>
       </c>
       <c r="D118" s="1" t="str">
         <f>_xlfn.XLOOKUP($A118,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PC14-OSC32_IN</v>
+        <v>PF15</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>683</v>
-      </c>
-      <c r="D119" s="1" t="str">
-        <f>_xlfn.XLOOKUP($A119,'UFBGA176+25 GPIOs'!$H$1:$H$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
-        <v>PF15</v>
-      </c>
+      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D120" s="1"/>
+      <c r="D120" t="s">
+        <v>353</v>
+      </c>
+      <c r="E120" t="s">
+        <v>354</v>
+      </c>
+      <c r="F120" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D121" t="s">
-        <v>353</v>
-      </c>
-      <c r="E121" t="s">
-        <v>354</v>
-      </c>
-      <c r="F121" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A121" t="s">
         <v>356</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C121" t="s">
         <v>762</v>
       </c>
-      <c r="D122" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",D$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="D121" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A121,"_",D$120),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>PA11</v>
       </c>
-      <c r="E122" s="1" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",E$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="E121" s="1" t="str">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A121,"_",E$120),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>PA12</v>
       </c>
-      <c r="F122" s="1" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A122,"_",F$121),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
+      <c r="F121" s="1" t="e">
+        <f>_xlfn.XLOOKUP(_xlfn.CONCAT($A121,"_",F$120),'UFBGA176+25 GPIOs'!$B$1:$B$133,'UFBGA176+25 GPIOs'!$A$1:$A$133)</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>712</v>
+      </c>
+      <c r="C123" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -6380,7 +6379,7 @@
         <v>712</v>
       </c>
       <c r="C124" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -6388,7 +6387,7 @@
         <v>712</v>
       </c>
       <c r="C125" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -6396,36 +6395,36 @@
         <v>712</v>
       </c>
       <c r="C126" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>712</v>
-      </c>
-      <c r="C127" t="s">
         <v>578</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>713</v>
+      </c>
+      <c r="C128" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C129" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C130" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C131" t="s">
         <v>129</v>
@@ -6433,41 +6432,33 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C132" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C133" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C134" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C135" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>720</v>
-      </c>
-      <c r="C136" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6482,8 +6473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0D7FC5-7D5B-4EB8-ACE9-BD3157D0914C}">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="73.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,13 +7908,13 @@
         <v>136</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>682</v>
+        <v>792</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>147</v>
       </c>
@@ -7946,7 +7937,7 @@
         <v>136</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>1</v>
@@ -10769,7 +10760,7 @@
         <v>462</v>
       </c>
       <c r="E36" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J36" t="s">
         <v>538</v>
@@ -10790,7 +10781,7 @@
         <v>463</v>
       </c>
       <c r="E37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J37" t="s">
         <v>538</v>
@@ -10801,7 +10792,7 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
@@ -10814,7 +10805,7 @@
         <v>450</v>
       </c>
       <c r="F38" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J38" t="s">
         <v>538</v>
@@ -10825,7 +10816,7 @@
         <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
@@ -10838,7 +10829,7 @@
         <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="J39" t="s">
         <v>538</v>
@@ -14680,7 +14671,7 @@
         <v>AMUX_EN</v>
       </c>
       <c r="C157" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -14689,7 +14680,7 @@
         <v>AMUX_A0</v>
       </c>
       <c r="C158" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -14698,7 +14689,7 @@
         <v>AMUX_A1</v>
       </c>
       <c r="C159" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>